<commit_message>
Allow depleted to be changed back to not depleted by the sample update template
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_update_v0.5.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_update_v0.5.xlsx
@@ -1515,7 +1515,7 @@
   <dimension ref="A1:H391"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6182,12 +6182,12 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G8:G391" type="list">
-      <formula1>"YES"</formula1>
+    <dataValidation allowBlank="true" operator="between" promptTitle="Coordinate" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C8:C391" type="list">
+      <formula1>Index!$B$2:$B$385</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" promptTitle="Coordinate" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C8:C391" type="list">
-      <formula1>Index!$B$2:$B$385</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G8:G391" type="list">
+      <formula1>"YES,NO"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>